<commit_message>
Added Excel Content New
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3b187250c9f36ea2/Desktop/Abhijit/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D4A151D4-7531-44A4-9B54-FEA3C1CACA31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{D4A151D4-7531-44A4-9B54-FEA3C1CACA31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{74EFA0A6-8602-4C72-8F40-3131C990559A}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{43728647-E090-45A7-B2D5-22104B751D18}"/>
   </bookViews>
@@ -410,10 +410,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA7EAE41-FEE4-4915-98E7-EF53BBAB89F2}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="A2" sqref="A2:A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -435,6 +435,11 @@
       </c>
       <c r="B2" s="1"/>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>45109</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>